<commit_message>
form data display to another page
</commit_message>
<xml_diff>
--- a/xam.xlsx
+++ b/xam.xlsx
@@ -405,7 +405,7 @@
   <dimension ref="A1:J15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M4" sqref="M4"/>
+      <selection activeCell="I15" sqref="I15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -471,6 +471,9 @@
       <c r="H2">
         <v>30</v>
       </c>
+      <c r="I2">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -497,6 +500,9 @@
       <c r="H3">
         <v>24</v>
       </c>
+      <c r="I3">
+        <v>86</v>
+      </c>
     </row>
     <row r="4" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -523,6 +529,9 @@
       <c r="H4">
         <v>32</v>
       </c>
+      <c r="I4">
+        <v>100</v>
+      </c>
     </row>
     <row r="5" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -549,6 +558,9 @@
       <c r="H5">
         <v>38</v>
       </c>
+      <c r="I5">
+        <v>112</v>
+      </c>
     </row>
     <row r="6" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -575,6 +587,9 @@
       <c r="H6">
         <v>40</v>
       </c>
+      <c r="I6">
+        <v>106</v>
+      </c>
     </row>
     <row r="7" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -601,6 +616,9 @@
       <c r="H7">
         <v>40</v>
       </c>
+      <c r="I7">
+        <v>114</v>
+      </c>
     </row>
     <row r="8" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A8">
@@ -627,6 +645,9 @@
       <c r="H8">
         <v>32</v>
       </c>
+      <c r="I8">
+        <v>86</v>
+      </c>
     </row>
     <row r="9" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A9">
@@ -653,6 +674,9 @@
       <c r="H9">
         <v>18</v>
       </c>
+      <c r="I9">
+        <v>72</v>
+      </c>
     </row>
     <row r="10" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -679,6 +703,9 @@
       <c r="H10">
         <v>38</v>
       </c>
+      <c r="I10">
+        <v>118</v>
+      </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -705,6 +732,9 @@
       <c r="H11">
         <v>38</v>
       </c>
+      <c r="I11">
+        <v>116</v>
+      </c>
     </row>
     <row r="12" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -731,6 +761,9 @@
       <c r="H12">
         <v>30</v>
       </c>
+      <c r="I12">
+        <v>106</v>
+      </c>
     </row>
     <row r="13" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -757,6 +790,9 @@
       <c r="H13">
         <v>30</v>
       </c>
+      <c r="I13">
+        <v>92</v>
+      </c>
     </row>
     <row r="14" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -783,6 +819,9 @@
       <c r="H14">
         <v>40</v>
       </c>
+      <c r="I14">
+        <v>100</v>
+      </c>
     </row>
     <row r="15" spans="1:10" x14ac:dyDescent="0.25">
       <c r="A15">
@@ -805,6 +844,9 @@
       </c>
       <c r="H15">
         <v>22</v>
+      </c>
+      <c r="I15">
+        <v>78</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
First Module Exam Result
</commit_message>
<xml_diff>
--- a/xam.xlsx
+++ b/xam.xlsx
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="21" uniqueCount="21">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
   <si>
     <t>Name</t>
   </si>
@@ -87,13 +87,22 @@
   </si>
   <si>
     <t>Sakil Mahbub</t>
+  </si>
+  <si>
+    <t>Total</t>
+  </si>
+  <si>
+    <t>evidence</t>
+  </si>
+  <si>
+    <t>Wriiten</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -101,13 +110,26 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FFFF0000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -122,9 +144,11 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="14" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -405,10 +429,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:K15"/>
+  <dimension ref="A1:S15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="K8" sqref="K8"/>
+    <sheetView tabSelected="1" topLeftCell="B1" workbookViewId="0">
+      <selection activeCell="K11" sqref="K11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -417,7 +441,7 @@
     <col min="7" max="7" width="9.7109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>1</v>
       </c>
@@ -445,11 +469,26 @@
       <c r="I1" t="s">
         <v>18</v>
       </c>
+      <c r="J1" t="s">
+        <v>22</v>
+      </c>
       <c r="K1" t="s">
+        <v>23</v>
+      </c>
+      <c r="L1" t="s">
+        <v>21</v>
+      </c>
+      <c r="Q1" t="s">
         <v>19</v>
       </c>
-    </row>
-    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R1" s="1">
+        <v>43227</v>
+      </c>
+      <c r="S1" s="1">
+        <v>43288</v>
+      </c>
+    </row>
+    <row r="2" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A2">
         <v>1244255</v>
       </c>
@@ -477,11 +516,27 @@
       <c r="I2">
         <v>92</v>
       </c>
+      <c r="J2">
+        <v>42</v>
+      </c>
       <c r="K2">
+        <v>74</v>
+      </c>
+      <c r="L2">
+        <f>SUM(C2:K2)</f>
+        <v>392.25</v>
+      </c>
+      <c r="Q2">
         <v>50</v>
       </c>
-    </row>
-    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R2">
+        <v>58</v>
+      </c>
+      <c r="S2">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="3" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A3">
         <v>1245212</v>
       </c>
@@ -509,11 +564,27 @@
       <c r="I3">
         <v>86</v>
       </c>
+      <c r="J3">
+        <v>44</v>
+      </c>
       <c r="K3">
+        <v>70</v>
+      </c>
+      <c r="L3">
+        <f>SUM(C3:K3)</f>
+        <v>370.5</v>
+      </c>
+      <c r="Q3">
         <v>30</v>
       </c>
-    </row>
-    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R3">
+        <v>50</v>
+      </c>
+      <c r="S3">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="4" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A4">
         <v>1244633</v>
       </c>
@@ -541,11 +612,27 @@
       <c r="I4">
         <v>100</v>
       </c>
+      <c r="J4">
+        <v>44</v>
+      </c>
       <c r="K4">
+        <v>70</v>
+      </c>
+      <c r="L4">
+        <f>SUM(C4:K4)</f>
+        <v>384.75</v>
+      </c>
+      <c r="Q4">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R4">
+        <v>62</v>
+      </c>
+      <c r="S4">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="5" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A5">
         <v>1243560</v>
       </c>
@@ -573,75 +660,123 @@
       <c r="I5">
         <v>112</v>
       </c>
+      <c r="J5">
+        <v>48</v>
+      </c>
       <c r="K5">
+        <v>78</v>
+      </c>
+      <c r="L5" s="3">
+        <f>SUM(C5:K5)</f>
+        <v>436.1</v>
+      </c>
+      <c r="Q5">
         <v>50</v>
       </c>
-    </row>
-    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R5">
+        <v>64</v>
+      </c>
+      <c r="S5">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="6" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A6">
         <v>1243288</v>
       </c>
-      <c r="B6" t="s">
+      <c r="B6" s="3" t="s">
         <v>3</v>
       </c>
-      <c r="C6">
+      <c r="C6" s="3">
         <v>9.5</v>
       </c>
-      <c r="D6">
+      <c r="D6" s="3">
         <v>27</v>
       </c>
-      <c r="E6">
+      <c r="E6" s="3">
         <v>11</v>
       </c>
-      <c r="F6">
+      <c r="F6" s="3">
         <v>85.5</v>
       </c>
-      <c r="G6">
-        <v>28</v>
-      </c>
-      <c r="H6">
+      <c r="G6" s="3">
+        <v>28</v>
+      </c>
+      <c r="H6" s="3">
         <v>40</v>
       </c>
-      <c r="I6">
+      <c r="I6" s="3">
         <v>106</v>
       </c>
-      <c r="K6">
+      <c r="J6" s="3">
+        <v>48</v>
+      </c>
+      <c r="K6" s="3">
+        <v>79</v>
+      </c>
+      <c r="L6" s="3">
+        <f>SUM(C6:K6)</f>
+        <v>434</v>
+      </c>
+      <c r="Q6">
         <v>50</v>
       </c>
-    </row>
-    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R6">
+        <v>60</v>
+      </c>
+      <c r="S6">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="7" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A7">
         <v>1243838</v>
       </c>
-      <c r="B7" t="s">
+      <c r="B7" s="3" t="s">
         <v>20</v>
       </c>
-      <c r="C7">
+      <c r="C7" s="3">
         <v>8.5</v>
       </c>
-      <c r="D7">
+      <c r="D7" s="3">
         <v>24.33</v>
       </c>
-      <c r="E7">
+      <c r="E7" s="3">
         <v>10</v>
       </c>
-      <c r="F7">
+      <c r="F7" s="3">
         <v>76.5</v>
       </c>
-      <c r="G7">
-        <v>28</v>
-      </c>
-      <c r="H7">
+      <c r="G7" s="3">
+        <v>28</v>
+      </c>
+      <c r="H7" s="3">
         <v>40</v>
       </c>
-      <c r="I7">
+      <c r="I7" s="3">
         <v>114</v>
       </c>
-      <c r="K7">
+      <c r="J7" s="3">
+        <v>44</v>
+      </c>
+      <c r="K7" s="3">
+        <v>70</v>
+      </c>
+      <c r="L7" s="3">
+        <f>SUM(C7:K7)</f>
+        <v>415.33</v>
+      </c>
+      <c r="Q7">
         <v>50</v>
       </c>
-    </row>
-    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R7">
+        <v>60</v>
+      </c>
+      <c r="S7">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="8" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A8">
         <v>1244244</v>
       </c>
@@ -670,10 +805,17 @@
         <v>86</v>
       </c>
       <c r="K8">
+        <v>58</v>
+      </c>
+      <c r="L8">
+        <f>SUM(C8:K8)</f>
+        <v>317.75</v>
+      </c>
+      <c r="Q8">
         <v>15</v>
       </c>
     </row>
-    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A9">
         <v>1244149</v>
       </c>
@@ -701,43 +843,75 @@
       <c r="I9">
         <v>72</v>
       </c>
+      <c r="J9">
+        <v>42</v>
+      </c>
       <c r="K9">
+        <v>84</v>
+      </c>
+      <c r="L9">
+        <f>SUM(C9:K9)</f>
+        <v>345.3</v>
+      </c>
+      <c r="Q9">
         <v>35</v>
       </c>
-    </row>
-    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R9">
+        <v>66</v>
+      </c>
+      <c r="S9">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="10" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A10">
         <v>1243564</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B10" s="3" t="s">
         <v>13</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="3" t="s">
         <v>9</v>
       </c>
-      <c r="D10">
+      <c r="D10" s="3">
         <v>30</v>
       </c>
-      <c r="E10">
+      <c r="E10" s="3">
         <v>11</v>
       </c>
-      <c r="F10">
+      <c r="F10" s="3">
         <v>81</v>
       </c>
-      <c r="G10">
-        <v>28</v>
-      </c>
-      <c r="H10">
+      <c r="G10" s="3">
+        <v>28</v>
+      </c>
+      <c r="H10" s="3">
         <v>38</v>
       </c>
-      <c r="I10">
+      <c r="I10" s="3">
         <v>118</v>
       </c>
-      <c r="K10">
+      <c r="J10" s="3">
+        <v>44</v>
+      </c>
+      <c r="K10" s="3">
+        <v>78</v>
+      </c>
+      <c r="L10" s="3">
+        <f>SUM(D10:K10)</f>
+        <v>428</v>
+      </c>
+      <c r="Q10">
         <v>50</v>
       </c>
-    </row>
-    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R10">
+        <v>64</v>
+      </c>
+      <c r="S10">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="11" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A11">
         <v>1244351</v>
       </c>
@@ -765,11 +939,24 @@
       <c r="I11">
         <v>116</v>
       </c>
-      <c r="K11">
+      <c r="J11">
+        <v>35</v>
+      </c>
+      <c r="L11">
+        <f>SUM(D11:K11)</f>
+        <v>310.5</v>
+      </c>
+      <c r="Q11">
         <v>0</v>
       </c>
-    </row>
-    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R11">
+        <v>58</v>
+      </c>
+      <c r="S11">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="12" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A12">
         <v>1243613</v>
       </c>
@@ -797,11 +984,27 @@
       <c r="I12">
         <v>106</v>
       </c>
+      <c r="J12">
+        <v>45</v>
+      </c>
       <c r="K12">
+        <v>72</v>
+      </c>
+      <c r="L12">
+        <f>SUM(C12:K12)</f>
+        <v>388.45</v>
+      </c>
+      <c r="Q12">
         <v>50</v>
       </c>
-    </row>
-    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R12">
+        <v>60</v>
+      </c>
+      <c r="S12">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="13" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A13">
         <v>1244155</v>
       </c>
@@ -829,11 +1032,27 @@
       <c r="I13">
         <v>92</v>
       </c>
+      <c r="J13">
+        <v>48</v>
+      </c>
       <c r="K13">
+        <v>76</v>
+      </c>
+      <c r="L13">
+        <f>SUM(C13:K13)</f>
+        <v>388.45</v>
+      </c>
+      <c r="Q13">
         <v>45</v>
       </c>
-    </row>
-    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R13">
+        <v>58</v>
+      </c>
+      <c r="S13">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="14" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A14">
         <v>1243859</v>
       </c>
@@ -861,11 +1080,27 @@
       <c r="I14">
         <v>100</v>
       </c>
+      <c r="J14">
+        <v>48</v>
+      </c>
       <c r="K14">
+        <v>90</v>
+      </c>
+      <c r="L14" s="2">
+        <f>SUM(C14:K14)</f>
+        <v>436.25</v>
+      </c>
+      <c r="Q14">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="R14">
+        <v>48</v>
+      </c>
+      <c r="S14">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="15" spans="1:19" x14ac:dyDescent="0.25">
       <c r="A15">
         <v>1244316</v>
       </c>
@@ -890,11 +1125,22 @@
       <c r="I15">
         <v>78</v>
       </c>
-      <c r="K15">
+      <c r="J15">
+        <v>42</v>
+      </c>
+      <c r="L15">
+        <f>SUM(C15:K15)</f>
+        <v>236.25</v>
+      </c>
+      <c r="Q15">
+        <v>0</v>
+      </c>
+      <c r="R15">
         <v>0</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
final  form eveidence for Js
</commit_message>
<xml_diff>
--- a/xam.xlsx
+++ b/xam.xlsx
@@ -1,20 +1,15 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="9302"/>
   <workbookPr/>
-  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
-    <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\J2EE-37\J2EE-Scholarship\"/>
-    </mc:Choice>
-  </mc:AlternateContent>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="15360" windowHeight="7650"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="144525"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -24,7 +19,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="24" uniqueCount="24">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="25" uniqueCount="25">
   <si>
     <t>Name</t>
   </si>
@@ -96,6 +91,9 @@
   </si>
   <si>
     <t>Wriiten</t>
+  </si>
+  <si>
+    <t>17/07/2018</t>
   </si>
 </sst>
 </file>
@@ -160,8 +158,36 @@
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
-  <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
+  <dxfs count="2">
+    <dxf>
+      <font>
+        <b/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFD7D7D7"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <font>
+        <b val="0"/>
+        <i val="0"/>
+      </font>
+      <fill>
+        <patternFill patternType="none">
+          <bgColor indexed="65"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
+  <tableStyles count="1" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16">
+    <tableStyle name="MySqlDefault" pivot="0" table="0" count="2">
+      <tableStyleElement type="wholeTable" dxfId="1"/>
+      <tableStyleElement type="headerRow" dxfId="0"/>
+    </tableStyle>
+  </tableStyles>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -216,7 +242,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -251,7 +277,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -428,7 +454,7 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns="" xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
@@ -439,7 +465,8 @@
   <dimension ref="A1:AD15"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="Q11" sqref="Q11"/>
+      <pane xSplit="1" topLeftCell="I1" activePane="topRight" state="frozen"/>
+      <selection pane="topRight" activeCell="S14" sqref="S14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -497,6 +524,9 @@
       <c r="Q1" s="1">
         <v>43319</v>
       </c>
+      <c r="R1" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="2" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A2">
@@ -548,6 +578,9 @@
       <c r="Q2">
         <v>140</v>
       </c>
+      <c r="R2">
+        <v>32</v>
+      </c>
     </row>
     <row r="3" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A3">
@@ -599,6 +632,9 @@
       <c r="Q3">
         <v>130</v>
       </c>
+      <c r="R3">
+        <v>32</v>
+      </c>
     </row>
     <row r="4" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A4">
@@ -650,6 +686,9 @@
       <c r="Q4">
         <v>162</v>
       </c>
+      <c r="R4">
+        <v>46</v>
+      </c>
     </row>
     <row r="5" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A5">
@@ -701,6 +740,9 @@
       <c r="Q5">
         <v>164</v>
       </c>
+      <c r="R5">
+        <v>46</v>
+      </c>
     </row>
     <row r="6" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A6">
@@ -752,6 +794,9 @@
       <c r="Q6">
         <v>156</v>
       </c>
+      <c r="R6">
+        <v>24</v>
+      </c>
     </row>
     <row r="7" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A7">
@@ -802,6 +847,9 @@
       </c>
       <c r="Q7">
         <v>158</v>
+      </c>
+      <c r="R7">
+        <v>32</v>
       </c>
     </row>
     <row r="8" spans="1:30" x14ac:dyDescent="0.25">
@@ -911,6 +959,9 @@
       <c r="Q9">
         <v>100</v>
       </c>
+      <c r="R9">
+        <v>44</v>
+      </c>
     </row>
     <row r="10" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A10">
@@ -962,6 +1013,9 @@
       <c r="Q10">
         <v>160</v>
       </c>
+      <c r="R10">
+        <v>62</v>
+      </c>
     </row>
     <row r="11" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A11">
@@ -1010,6 +1064,9 @@
       <c r="Q11">
         <v>150</v>
       </c>
+      <c r="R11">
+        <v>18</v>
+      </c>
     </row>
     <row r="12" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A12">
@@ -1061,6 +1118,9 @@
       <c r="Q12">
         <v>164</v>
       </c>
+      <c r="R12">
+        <v>48</v>
+      </c>
     </row>
     <row r="13" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A13">
@@ -1112,6 +1172,9 @@
       <c r="Q13">
         <v>142</v>
       </c>
+      <c r="R13">
+        <v>40</v>
+      </c>
     </row>
     <row r="14" spans="1:30" x14ac:dyDescent="0.25">
       <c r="A14">
@@ -1162,6 +1225,9 @@
       </c>
       <c r="Q14">
         <v>158</v>
+      </c>
+      <c r="R14">
+        <v>38</v>
       </c>
     </row>
     <row r="15" spans="1:30" x14ac:dyDescent="0.25">

</xml_diff>